<commit_message>
Testing for AI shouldn't pass too close to the net so often (4REV29H4)
Experimented with different solutions and think I came up with a good mix!
</commit_message>
<xml_diff>
--- a/Resources/GetTimeForSpike debugging.xlsx
+++ b/Resources/GetTimeForSpike debugging.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74F7BD88-9FE0-41B3-AC7A-6095E1F5007F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5B0907-50E8-4BE1-B6B5-84C9380FBB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{53CC6AC9-9577-45F0-AF66-7F38B62D387C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>spikepos</t>
   </si>
@@ -188,13 +188,163 @@
     <t>For example:</t>
   </si>
   <si>
-    <r>
+    <t>2. Incorrect Parameters for the Arc:</t>
+  </si>
+  <si>
+    <t>3. Floating-Point Precision Issues:</t>
+  </si>
+  <si>
+    <t>This is less common but can happen with very small arcs or specific edge cases.</t>
+  </si>
+  <si>
+    <t>4. Timing Issues:</t>
+  </si>
+  <si>
+    <t>apex</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Due to floating-point rounding errors, values of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> could result in a slightly negative discriminant when it should be zero.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Logic for Valid Solutions (Range of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The function considers solutions only if ttt is between 0.5 and 1 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>t1 &gt;= 0.5f &amp;&amp; t1 &lt;= 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>). If both solutions fall outside this range, you'll get no valid result.</t>
+    </r>
+  </si>
+  <si>
+    <t>b^2</t>
+  </si>
+  <si>
+    <t>4ac</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the arc isn't physically achievable, certain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
       <t>spikePos</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> values will not be reachable.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>spikePos</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -203,16 +353,18 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>height + start</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -226,8 +378,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -236,16 +389,18 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>start</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -254,28 +409,12 @@
     </r>
   </si>
   <si>
-    <t>2. Incorrect Parameters for the Arc:</t>
-  </si>
-  <si>
-    <t>3. Floating-Point Precision Issues:</t>
-  </si>
-  <si>
-    <t>This is less common but can happen with very small arcs or specific edge cases.</t>
-  </si>
-  <si>
-    <t>4. Timing Issues:</t>
-  </si>
-  <si>
-    <t>apex</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">The parameters </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>start</t>
@@ -283,7 +422,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -293,7 +431,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>end</t>
@@ -301,7 +438,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -311,7 +447,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>height</t>
@@ -319,7 +454,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -329,7 +463,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>duration</t>
@@ -337,58 +470,51 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> might not define a valid arc (e.g., height is too small or negative, or </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>start</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>end</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> are too far apart for the given duration).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If the arc isn't physically achievable, certain </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> might not define a valid arc</t>
+    </r>
+  </si>
+  <si>
+    <t>height is too small or negative</t>
+  </si>
+  <si>
+    <t>start and end are too far apart for the given duration</t>
+  </si>
+  <si>
+    <t>too small?</t>
+  </si>
+  <si>
+    <t>start-end</t>
+  </si>
+  <si>
+    <t>too far?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>duration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> parameter is too short for the ball to reach </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>spikePos</t>
@@ -396,107 +522,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> values will not be reachable.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Due to floating-point rounding errors, values of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, or </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> could result in a slightly negative discriminant when it should be zero.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>duration</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> parameter is too short for the ball to reach </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>spikePos</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -506,7 +531,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Arial Unicode MS"/>
       </rPr>
       <t>t</t>
@@ -514,60 +538,11 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> solutions.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. Logic for Valid Solutions (Range of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>):</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>The function considers solutions only if ttt is between 0.5 and 1 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>t1 &gt;= 0.5f &amp;&amp; t1 &lt;= 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.249977111117893"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>). If both solutions fall outside this range, you'll get no valid result.</t>
     </r>
   </si>
 </sst>
@@ -575,7 +550,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +611,37 @@
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -657,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -668,20 +674,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1026,18 +1069,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052FB0CA-ADCE-405D-9C09-993B954BE7CB}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,23 +1089,23 @@
         <v>4.1944730000000003</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>3.467301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.5043920000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>1.2505980000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1069,75 +1113,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.50555559999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>1.823976</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <f>-4*B2</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>-13.869204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <f>4*B2-B3+B4</f>
-        <v>-7.5043920000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>12.618606</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <f>B3-B1</f>
-        <v>-0.69008100000000017</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>-2.9438750000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <f>B8*B8-4*B7*B9</f>
-        <v>67.357195289664006</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>-4.0875943187640189</v>
+      </c>
+      <c r="D11">
+        <f>B8^2</f>
+        <v>159.229217383236</v>
+      </c>
+      <c r="E11">
+        <f>4*B7*B9</f>
+        <v>163.31681170200002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
-        <f>SQRT(B11)</f>
-        <v>8.2071429431723679</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" t="str">
+        <f>IFERROR(SQRT(B11),"No real solution")</f>
+        <v>No real solution</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
-        <f>(-B8+B13)/(2*B7)</f>
-        <v>1.9639418678965459</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="B14" t="str">
+        <f>IFERROR((-B8+B13)/(2*B7),"No real solution")</f>
+        <v>No real solution</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
-        <f>(-B8-B13)/(2*B7)</f>
-        <v>-8.7843867896545968E-2</v>
+      <c r="B15" t="str">
+        <f>IFERROR((-B8-B13)/(2*B7),"No real solution")</f>
+        <v>No real solution</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1145,8 +1205,8 @@
         <v>12</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(AND(B14&gt;=0.5,B14&lt;=1),B14,"")</f>
-        <v/>
+        <f>IF(AND(B14&gt;=0.5,B14&lt;=1),B14,"can't")</f>
+        <v>can't</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1154,8 +1214,8 @@
         <v>13</v>
       </c>
       <c r="B18" t="str">
-        <f>IF(AND(B15&gt;=0.5,B15&lt;=1),B15,"")</f>
-        <v/>
+        <f>IF(AND(B15&gt;=0.5,B15&lt;=1),B15,"can't")</f>
+        <v>can't</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="18">
@@ -1179,8 +1239,8 @@
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="4" t="s">
-        <v>18</v>
+      <c r="A24" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -1190,16 +1250,16 @@
         <v>4.1944730000000003</v>
       </c>
       <c r="J24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K24">
         <f>B2+B3</f>
-        <v>2.5043920000000002</v>
+        <v>4.7178990000000001</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="4" t="s">
-        <v>19</v>
+      <c r="A25" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="H25" t="s">
         <v>0</v>
@@ -1213,68 +1273,119 @@
       </c>
       <c r="K25">
         <f>B3</f>
-        <v>3.5043920000000002</v>
+        <v>1.2505980000000001</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
+      <c r="A26" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="6" t="s">
-        <v>25</v>
+      <c r="A27" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="6" t="s">
-        <v>26</v>
+      <c r="A28" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="5" t="s">
-        <v>21</v>
+      <c r="A29" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f>B2</f>
+        <v>3.467301</v>
+      </c>
+      <c r="J29" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29">
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="6" t="s">
-        <v>27</v>
+      <c r="A30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30">
+        <f>ABS(B3-B4)</f>
+        <v>1.2505980000000001</v>
+      </c>
+      <c r="J30" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="6" t="s">
-        <v>22</v>
+      <c r="A31" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="6" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>I24&gt;K24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>I25&lt;K25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>I29&lt;K29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>I25&lt;K25</formula>
+      <formula>I30&gt;K30</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>